<commit_message>
Add creation of add-on file to run with fixed quantity trade between NEMS regions.  Have an advanced electric cars scenario.  Also bug fixes which includes: fix HDD/CDD to the base year value to be consisten with the Core methodology.  Changing HDD/CDD should vary to match the scenario being run such as A2, B1.  Allow states that did not have wind in the base year have it in the future.  The subsector level logit in industry was being read in the wrong column and therefore being set as the share-weight in the XML. Some near term share-weights for electricity were adjusted to match what is currently being done at the USA level.
</commit_message>
<xml_diff>
--- a/rgcam-data-system/rgcam-data/Assumptions/Tables_Trn_Data.xlsx
+++ b/rgcam-data-system/rgcam-data/Assumptions/Tables_Trn_Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,10 @@
     <sheet name="A_trn_tech_interp" sheetId="6" r:id="rId7"/>
     <sheet name="A_trn_tech_input" sheetId="7" r:id="rId8"/>
     <sheet name="A_trn_finaldemand" sheetId="8" r:id="rId9"/>
+    <sheet name="A_trn_elec_adv" sheetId="10" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="66">
   <si>
     <t>This workbook collects transportation assumptions from the global detailed transportation workbook and reorganizes it into table readily usable in the R processing</t>
   </si>
@@ -226,6 +227,9 @@
   <si>
     <t>Proc_name</t>
   </si>
+  <si>
+    <t># Assumed technology charactoristics including costs and efficiencies for advanced electric vehicles scenario</t>
+  </si>
 </sst>
 </file>
 
@@ -327,7 +331,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="510">
+  <cellStyleXfs count="544">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -350,6 +354,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -854,7 +892,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="510">
+  <cellStyles count="544">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1109,6 +1147,23 @@
     <cellStyle name="Followed Hyperlink" xfId="505" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="507" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="509" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1363,6 +1418,23 @@
     <cellStyle name="Hyperlink" xfId="504" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="506" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="508" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="510" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="21"/>
   </cellStyles>
@@ -5014,7 +5086,2035 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="11">
+        <row r="24">
+          <cell r="F24">
+            <v>1975</v>
+          </cell>
+          <cell r="G24">
+            <v>1990</v>
+          </cell>
+          <cell r="H24">
+            <v>2005</v>
+          </cell>
+          <cell r="I24">
+            <v>2020</v>
+          </cell>
+          <cell r="J24">
+            <v>2035</v>
+          </cell>
+          <cell r="K24">
+            <v>2050</v>
+          </cell>
+          <cell r="L24">
+            <v>2065</v>
+          </cell>
+          <cell r="M24">
+            <v>2080</v>
+          </cell>
+          <cell r="N24">
+            <v>2095</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>trn_freight</v>
+          </cell>
+          <cell r="D25" t="str">
+            <v>air</v>
+          </cell>
+          <cell r="F25">
+            <v>199239.20974871737</v>
+          </cell>
+          <cell r="G25">
+            <v>199239.20974871737</v>
+          </cell>
+          <cell r="H25">
+            <v>199239.20974871737</v>
+          </cell>
+          <cell r="I25">
+            <v>177964.15712635888</v>
+          </cell>
+          <cell r="J25">
+            <v>158960.88556885699</v>
+          </cell>
+          <cell r="K25">
+            <v>141986.81098966434</v>
+          </cell>
+          <cell r="L25">
+            <v>126825.25278384826</v>
+          </cell>
+          <cell r="M25">
+            <v>113282.66781664576</v>
+          </cell>
+          <cell r="N25">
+            <v>101186.1797707439</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v>trn_freight</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>rail ICE</v>
+          </cell>
+          <cell r="F26">
+            <v>8737.8928058855199</v>
+          </cell>
+          <cell r="G26">
+            <v>8737.8928058855199</v>
+          </cell>
+          <cell r="H26">
+            <v>8737.8928058855199</v>
+          </cell>
+          <cell r="I26">
+            <v>8415.8944102173427</v>
+          </cell>
+          <cell r="J26">
+            <v>8105.7619150718911</v>
+          </cell>
+          <cell r="K26">
+            <v>7807.0580524468733</v>
+          </cell>
+          <cell r="L26">
+            <v>7519.3616680184705</v>
+          </cell>
+          <cell r="M26">
+            <v>7242.2671273392934</v>
+          </cell>
+          <cell r="N26">
+            <v>6975.3837439184208</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v>trn_freight</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>rail electric</v>
+          </cell>
+          <cell r="F27">
+            <v>2950.457311078228</v>
+          </cell>
+          <cell r="G27">
+            <v>2950.457311078228</v>
+          </cell>
+          <cell r="H27">
+            <v>2950.457311078228</v>
+          </cell>
+          <cell r="I27">
+            <v>2841.7305800733889</v>
+          </cell>
+          <cell r="J27">
+            <v>2737.0105167775223</v>
+          </cell>
+          <cell r="K27">
+            <v>2636.1494722547891</v>
+          </cell>
+          <cell r="L27">
+            <v>2539.0052385516919</v>
+          </cell>
+          <cell r="M27">
+            <v>2445.4408481924893</v>
+          </cell>
+          <cell r="N27">
+            <v>2355.3243810633635</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>trn_freight</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>truck ICE</v>
+          </cell>
+          <cell r="F28">
+            <v>12008.042580674342</v>
+          </cell>
+          <cell r="G28">
+            <v>12008.042580674342</v>
+          </cell>
+          <cell r="H28">
+            <v>12008.042580674342</v>
+          </cell>
+          <cell r="I28">
+            <v>10485.207670213153</v>
+          </cell>
+          <cell r="J28">
+            <v>9155.4955063561065</v>
+          </cell>
+          <cell r="K28">
+            <v>7994.414665246476</v>
+          </cell>
+          <cell r="L28">
+            <v>6980.5796743102128</v>
+          </cell>
+          <cell r="M28">
+            <v>6095.317121993512</v>
+          </cell>
+          <cell r="N28">
+            <v>5322.3217198417751</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v>trn_freight</v>
+          </cell>
+          <cell r="D29" t="str">
+            <v>domestic ship ICE</v>
+          </cell>
+          <cell r="F29">
+            <v>294105.06571153644</v>
+          </cell>
+          <cell r="G29">
+            <v>294105.06571153644</v>
+          </cell>
+          <cell r="H29">
+            <v>294105.06571153644</v>
+          </cell>
+          <cell r="I29">
+            <v>283267.05688940815</v>
+          </cell>
+          <cell r="J29">
+            <v>272828.43743156828</v>
+          </cell>
+          <cell r="K29">
+            <v>262774.48951789649</v>
+          </cell>
+          <cell r="L29">
+            <v>253091.03769181151</v>
+          </cell>
+          <cell r="M29">
+            <v>243764.42887373749</v>
+          </cell>
+          <cell r="N29">
+            <v>234781.51311109003</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v>trn_passenger</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v>air</v>
+          </cell>
+          <cell r="F30">
+            <v>199239.2097487174</v>
+          </cell>
+          <cell r="G30">
+            <v>199239.2097487174</v>
+          </cell>
+          <cell r="H30">
+            <v>199239.2097487174</v>
+          </cell>
+          <cell r="I30">
+            <v>177964.15712635891</v>
+          </cell>
+          <cell r="J30">
+            <v>158960.88556885699</v>
+          </cell>
+          <cell r="K30">
+            <v>141986.81098966434</v>
+          </cell>
+          <cell r="L30">
+            <v>126825.25278384826</v>
+          </cell>
+          <cell r="M30">
+            <v>113282.66781664576</v>
+          </cell>
+          <cell r="N30">
+            <v>101186.1797707439</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31" t="str">
+            <v>trn_passenger</v>
+          </cell>
+          <cell r="D31" t="str">
+            <v>high speed rail</v>
+          </cell>
+          <cell r="F31">
+            <v>113626.02960713686</v>
+          </cell>
+          <cell r="G31">
+            <v>113626.02960713686</v>
+          </cell>
+          <cell r="H31">
+            <v>113626.02960713686</v>
+          </cell>
+          <cell r="I31">
+            <v>109438.81879413639</v>
+          </cell>
+          <cell r="J31">
+            <v>105405.91007593874</v>
+          </cell>
+          <cell r="K31">
+            <v>101521.61729592942</v>
+          </cell>
+          <cell r="L31">
+            <v>97780.463836950235</v>
+          </cell>
+          <cell r="M31">
+            <v>94177.17489960129</v>
+          </cell>
+          <cell r="N31">
+            <v>90706.670065093916</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32" t="str">
+            <v>trn_passenger</v>
+          </cell>
+          <cell r="D32" t="str">
+            <v>rail ICE</v>
+          </cell>
+          <cell r="F32">
+            <v>30105.713316171692</v>
+          </cell>
+          <cell r="G32">
+            <v>30105.713316171692</v>
+          </cell>
+          <cell r="H32">
+            <v>30105.713316171692</v>
+          </cell>
+          <cell r="I32">
+            <v>28996.293504827263</v>
+          </cell>
+          <cell r="J32">
+            <v>27927.756708107914</v>
+          </cell>
+          <cell r="K32">
+            <v>26898.596353958823</v>
+          </cell>
+          <cell r="L32">
+            <v>25907.361388720215</v>
+          </cell>
+          <cell r="M32">
+            <v>24952.654231229724</v>
+          </cell>
+          <cell r="N32">
+            <v>24033.128802317751</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33" t="str">
+            <v>trn_passenger</v>
+          </cell>
+          <cell r="D33" t="str">
+            <v>rail electric</v>
+          </cell>
+          <cell r="F33">
+            <v>14548.862009235923</v>
+          </cell>
+          <cell r="G33">
+            <v>14548.862009235923</v>
+          </cell>
+          <cell r="H33">
+            <v>14548.862009235923</v>
+          </cell>
+          <cell r="I33">
+            <v>14012.724712768266</v>
+          </cell>
+          <cell r="J33">
+            <v>13496.344507987997</v>
+          </cell>
+          <cell r="K33">
+            <v>12998.99333013537</v>
+          </cell>
+          <cell r="L33">
+            <v>12519.969944224109</v>
+          </cell>
+          <cell r="M33">
+            <v>12058.598956342619</v>
+          </cell>
+          <cell r="N33">
+            <v>11614.229861389551</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>trn_shipping_intl</v>
+          </cell>
+          <cell r="D34" t="str">
+            <v>international ship ICE</v>
+          </cell>
+          <cell r="F34">
+            <v>2013405.2468509991</v>
+          </cell>
+          <cell r="G34">
+            <v>2013405.2468509991</v>
+          </cell>
+          <cell r="H34">
+            <v>2013405.2468509991</v>
+          </cell>
+          <cell r="I34">
+            <v>1939209.6400018018</v>
+          </cell>
+          <cell r="J34">
+            <v>1867748.2010923824</v>
+          </cell>
+          <cell r="K34">
+            <v>1798920.1738294726</v>
+          </cell>
+          <cell r="L34">
+            <v>1732628.514870456</v>
+          </cell>
+          <cell r="M34">
+            <v>1668779.7569981415</v>
+          </cell>
+          <cell r="N34">
+            <v>1607283.877337659</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v>LDV ICE</v>
+          </cell>
+          <cell r="F35">
+            <v>3607.1937941448978</v>
+          </cell>
+          <cell r="G35">
+            <v>3607.1937941448978</v>
+          </cell>
+          <cell r="H35">
+            <v>3607.1937941448987</v>
+          </cell>
+          <cell r="I35">
+            <v>2986.9368416834895</v>
+          </cell>
+          <cell r="J35">
+            <v>2473.3330686828513</v>
+          </cell>
+          <cell r="K35">
+            <v>2048.0434615391032</v>
+          </cell>
+          <cell r="L35">
+            <v>1721.8260468866938</v>
+          </cell>
+          <cell r="M35">
+            <v>1447.5693467508256</v>
+          </cell>
+          <cell r="N35">
+            <v>1226.2633600345937</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>LDV electric</v>
+          </cell>
+          <cell r="F36">
+            <v>1202.3979313816326</v>
+          </cell>
+          <cell r="G36">
+            <v>1202.3979313816326</v>
+          </cell>
+          <cell r="H36">
+            <v>1202.397931381633</v>
+          </cell>
+          <cell r="I36">
+            <v>1132.2394866886907</v>
+          </cell>
+          <cell r="J36">
+            <v>1066.1747012022947</v>
+          </cell>
+          <cell r="K36">
+            <v>1003.9647149281467</v>
+          </cell>
+          <cell r="L36">
+            <v>945.38460505968101</v>
+          </cell>
+          <cell r="M36">
+            <v>890.22257276025334</v>
+          </cell>
+          <cell r="N36">
+            <v>838.27917739559041</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>LDV gas</v>
+          </cell>
+          <cell r="F37">
+            <v>3607.1937941448978</v>
+          </cell>
+          <cell r="G37">
+            <v>3607.1937941448978</v>
+          </cell>
+          <cell r="H37">
+            <v>3607.1937941448987</v>
+          </cell>
+          <cell r="I37">
+            <v>2986.9368416834895</v>
+          </cell>
+          <cell r="J37">
+            <v>2473.3330686828513</v>
+          </cell>
+          <cell r="K37">
+            <v>2048.0434615391032</v>
+          </cell>
+          <cell r="L37">
+            <v>1721.8260468866938</v>
+          </cell>
+          <cell r="M37">
+            <v>1447.5693467508256</v>
+          </cell>
+          <cell r="N37">
+            <v>1226.2633600345937</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D38" t="str">
+            <v>LDV fuel cell</v>
+          </cell>
+          <cell r="F38">
+            <v>2284.5560696251018</v>
+          </cell>
+          <cell r="G38">
+            <v>2284.5560696251018</v>
+          </cell>
+          <cell r="H38">
+            <v>2284.5560696251023</v>
+          </cell>
+          <cell r="I38">
+            <v>1891.7266663995433</v>
+          </cell>
+          <cell r="J38">
+            <v>1566.4442768324725</v>
+          </cell>
+          <cell r="K38">
+            <v>1297.0941923080986</v>
+          </cell>
+          <cell r="L38">
+            <v>1074.0588532912959</v>
+          </cell>
+          <cell r="M38">
+            <v>996.26366299760321</v>
+          </cell>
+          <cell r="N38">
+            <v>924.10325855785709</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>bus ICE</v>
+          </cell>
+          <cell r="F39">
+            <v>15100.858196573312</v>
+          </cell>
+          <cell r="G39">
+            <v>15100.858196573312</v>
+          </cell>
+          <cell r="H39">
+            <v>15100.85819657331</v>
+          </cell>
+          <cell r="I39">
+            <v>12504.265715248419</v>
+          </cell>
+          <cell r="J39">
+            <v>10354.15729637257</v>
+          </cell>
+          <cell r="K39">
+            <v>8573.7600079378553</v>
+          </cell>
+          <cell r="L39">
+            <v>7099.5020231600565</v>
+          </cell>
+          <cell r="M39">
+            <v>6585.2777707462074</v>
+          </cell>
+          <cell r="N39">
+            <v>6108.2993111933174</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>bus electric</v>
+          </cell>
+          <cell r="F40">
+            <v>5033.6193988577706</v>
+          </cell>
+          <cell r="G40">
+            <v>5033.6193988577706</v>
+          </cell>
+          <cell r="H40">
+            <v>5033.6193988577697</v>
+          </cell>
+          <cell r="I40">
+            <v>4739.9138800913734</v>
+          </cell>
+          <cell r="J40">
+            <v>4463.3457181488593</v>
+          </cell>
+          <cell r="K40">
+            <v>4202.9149692765559</v>
+          </cell>
+          <cell r="L40">
+            <v>3957.6800352125033</v>
+          </cell>
+          <cell r="M40">
+            <v>3726.754258798564</v>
+          </cell>
+          <cell r="N40">
+            <v>3509.3027182343949</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>bus gas</v>
+          </cell>
+          <cell r="F41">
+            <v>15100.858196573312</v>
+          </cell>
+          <cell r="G41">
+            <v>15100.858196573312</v>
+          </cell>
+          <cell r="H41">
+            <v>40974.011764189789</v>
+          </cell>
+          <cell r="I41">
+            <v>33928.53067353525</v>
+          </cell>
+          <cell r="J41">
+            <v>28094.520016492334</v>
+          </cell>
+          <cell r="K41">
+            <v>23263.667458866868</v>
+          </cell>
+          <cell r="L41">
+            <v>19263.479971148878</v>
+          </cell>
+          <cell r="M41">
+            <v>15951.124699275109</v>
+          </cell>
+          <cell r="N41">
+            <v>13208.328897629066</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v>trn_pass_road</v>
+          </cell>
+          <cell r="D42" t="str">
+            <v>bus fuel cell</v>
+          </cell>
+          <cell r="F42">
+            <v>9563.876857829764</v>
+          </cell>
+          <cell r="G42">
+            <v>9563.876857829764</v>
+          </cell>
+          <cell r="H42">
+            <v>9563.8768578297622</v>
+          </cell>
+          <cell r="I42">
+            <v>7919.3682863239983</v>
+          </cell>
+          <cell r="J42">
+            <v>6557.6329543692937</v>
+          </cell>
+          <cell r="K42">
+            <v>5430.0480050273072</v>
+          </cell>
+          <cell r="L42">
+            <v>4496.3512813347015</v>
+          </cell>
+          <cell r="M42">
+            <v>3723.2037039898219</v>
+          </cell>
+          <cell r="N42">
+            <v>3082.9988481880014</v>
+          </cell>
+        </row>
+        <row r="322">
+          <cell r="E322">
+            <v>1990</v>
+          </cell>
+          <cell r="F322">
+            <v>2005</v>
+          </cell>
+          <cell r="G322">
+            <v>2020</v>
+          </cell>
+          <cell r="H322">
+            <v>2035</v>
+          </cell>
+          <cell r="I322">
+            <v>2050</v>
+          </cell>
+          <cell r="J322">
+            <v>2065</v>
+          </cell>
+          <cell r="K322">
+            <v>2080</v>
+          </cell>
+          <cell r="L322">
+            <v>2095</v>
+          </cell>
+        </row>
+        <row r="323">
+          <cell r="E323">
+            <v>8.215657298859437</v>
+          </cell>
+          <cell r="F323">
+            <v>8.215657298859437</v>
+          </cell>
+          <cell r="G323">
+            <v>8.215657298859437</v>
+          </cell>
+          <cell r="H323">
+            <v>8.215657298859437</v>
+          </cell>
+          <cell r="I323">
+            <v>8.215657298859437</v>
+          </cell>
+          <cell r="J323">
+            <v>8.215657298859437</v>
+          </cell>
+          <cell r="K323">
+            <v>8.215657298859437</v>
+          </cell>
+          <cell r="L323">
+            <v>8.215657298859437</v>
+          </cell>
+        </row>
+        <row r="324">
+          <cell r="E324">
+            <v>0.43713651555825689</v>
+          </cell>
+          <cell r="F324">
+            <v>0.43713651555825689</v>
+          </cell>
+          <cell r="G324">
+            <v>0.43713651555825689</v>
+          </cell>
+          <cell r="H324">
+            <v>0.43713651555825689</v>
+          </cell>
+          <cell r="I324">
+            <v>0.43713651555825689</v>
+          </cell>
+          <cell r="J324">
+            <v>0.43713651555825689</v>
+          </cell>
+          <cell r="K324">
+            <v>0.43713651555825689</v>
+          </cell>
+          <cell r="L324">
+            <v>0.43713651555825689</v>
+          </cell>
+        </row>
+        <row r="325">
+          <cell r="E325">
+            <v>0.48085016711408263</v>
+          </cell>
+          <cell r="F325">
+            <v>0.48085016711408263</v>
+          </cell>
+          <cell r="G325">
+            <v>0.45279314957056366</v>
+          </cell>
+          <cell r="H325">
+            <v>0.43283983453669406</v>
+          </cell>
+          <cell r="I325">
+            <v>0.43283983453669406</v>
+          </cell>
+          <cell r="J325">
+            <v>0.43283983453669406</v>
+          </cell>
+          <cell r="K325">
+            <v>0.43283983453669406</v>
+          </cell>
+          <cell r="L325">
+            <v>0.43283983453669406</v>
+          </cell>
+        </row>
+        <row r="326">
+          <cell r="E326">
+            <v>0.55044266747162252</v>
+          </cell>
+          <cell r="F326">
+            <v>0.55044266747162252</v>
+          </cell>
+          <cell r="G326">
+            <v>0.55044266747162252</v>
+          </cell>
+          <cell r="H326">
+            <v>0.55044266747162252</v>
+          </cell>
+          <cell r="I326">
+            <v>0.55044266747162252</v>
+          </cell>
+          <cell r="J326">
+            <v>0.55044266747162252</v>
+          </cell>
+          <cell r="K326">
+            <v>0.55044266747162252</v>
+          </cell>
+          <cell r="L326">
+            <v>0.55044266747162252</v>
+          </cell>
+        </row>
+        <row r="327">
+          <cell r="E327">
+            <v>2.2362592509925516</v>
+          </cell>
+          <cell r="F327">
+            <v>2.2362592509925516</v>
+          </cell>
+          <cell r="G327">
+            <v>2.2362592509925516</v>
+          </cell>
+          <cell r="H327">
+            <v>2.2362592509925516</v>
+          </cell>
+          <cell r="I327">
+            <v>2.2362592509925516</v>
+          </cell>
+          <cell r="J327">
+            <v>2.2362592509925516</v>
+          </cell>
+          <cell r="K327">
+            <v>2.2362592509925516</v>
+          </cell>
+          <cell r="L327">
+            <v>2.2362592509925516</v>
+          </cell>
+        </row>
+        <row r="328">
+          <cell r="E328">
+            <v>6.0272087942357908</v>
+          </cell>
+          <cell r="F328">
+            <v>6.0272087942357908</v>
+          </cell>
+          <cell r="G328">
+            <v>6.0272087942357908</v>
+          </cell>
+          <cell r="H328">
+            <v>6.0272087942357908</v>
+          </cell>
+          <cell r="I328">
+            <v>6.0272087942357908</v>
+          </cell>
+          <cell r="J328">
+            <v>6.0272087942357908</v>
+          </cell>
+          <cell r="K328">
+            <v>6.0272087942357908</v>
+          </cell>
+          <cell r="L328">
+            <v>6.0272087942357908</v>
+          </cell>
+        </row>
+        <row r="329">
+          <cell r="E329">
+            <v>31.475836601545215</v>
+          </cell>
+          <cell r="F329">
+            <v>31.475836601545215</v>
+          </cell>
+          <cell r="G329">
+            <v>31.0069897367297</v>
+          </cell>
+          <cell r="H329">
+            <v>30.545126558652367</v>
+          </cell>
+          <cell r="I329">
+            <v>30.090143042131182</v>
+          </cell>
+          <cell r="J329">
+            <v>29.641936711486391</v>
+          </cell>
+          <cell r="K329">
+            <v>29.200406617459976</v>
+          </cell>
+          <cell r="L329">
+            <v>28.765453314478911</v>
+          </cell>
+        </row>
+        <row r="330">
+          <cell r="E330">
+            <v>2.1310988398652362</v>
+          </cell>
+          <cell r="F330">
+            <v>2.1310988398652362</v>
+          </cell>
+          <cell r="G330">
+            <v>2.1310988398652362</v>
+          </cell>
+          <cell r="H330">
+            <v>2.1310988398652362</v>
+          </cell>
+          <cell r="I330">
+            <v>2.1310988398652362</v>
+          </cell>
+          <cell r="J330">
+            <v>2.1310988398652362</v>
+          </cell>
+          <cell r="K330">
+            <v>2.1310988398652362</v>
+          </cell>
+          <cell r="L330">
+            <v>2.1310988398652362</v>
+          </cell>
+        </row>
+        <row r="331">
+          <cell r="E331">
+            <v>1.759574734708778</v>
+          </cell>
+          <cell r="F331">
+            <v>1.759574734708778</v>
+          </cell>
+          <cell r="G331">
+            <v>1.759574734708778</v>
+          </cell>
+          <cell r="H331">
+            <v>1.759574734708778</v>
+          </cell>
+          <cell r="I331">
+            <v>1.759574734708778</v>
+          </cell>
+          <cell r="J331">
+            <v>1.759574734708778</v>
+          </cell>
+          <cell r="K331">
+            <v>1.759574734708778</v>
+          </cell>
+          <cell r="L331">
+            <v>1.759574734708778</v>
+          </cell>
+        </row>
+        <row r="332">
+          <cell r="E332">
+            <v>52.784967378763007</v>
+          </cell>
+          <cell r="F332">
+            <v>52.784967378763007</v>
+          </cell>
+          <cell r="G332">
+            <v>52.784967378763007</v>
+          </cell>
+          <cell r="H332">
+            <v>52.784967378763007</v>
+          </cell>
+          <cell r="I332">
+            <v>52.784967378763007</v>
+          </cell>
+          <cell r="J332">
+            <v>52.784967378763007</v>
+          </cell>
+          <cell r="K332">
+            <v>52.784967378763007</v>
+          </cell>
+          <cell r="L332">
+            <v>52.784967378763007</v>
+          </cell>
+        </row>
+        <row r="333">
+          <cell r="E333">
+            <v>0.25796421379738965</v>
+          </cell>
+          <cell r="F333">
+            <v>0.25796421379738965</v>
+          </cell>
+          <cell r="G333">
+            <v>0.25796421379738965</v>
+          </cell>
+          <cell r="H333">
+            <v>0.25796421379738965</v>
+          </cell>
+          <cell r="I333">
+            <v>0.25796421379738965</v>
+          </cell>
+          <cell r="J333">
+            <v>0.25796421379738965</v>
+          </cell>
+          <cell r="K333">
+            <v>0.25796421379738965</v>
+          </cell>
+          <cell r="L333">
+            <v>0.25796421379738965</v>
+          </cell>
+        </row>
+        <row r="334">
+          <cell r="E334">
+            <v>0.28376063517712863</v>
+          </cell>
+          <cell r="F334">
+            <v>0.28376063517712863</v>
+          </cell>
+          <cell r="G334">
+            <v>0.27125610556295471</v>
+          </cell>
+          <cell r="H334">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="I334">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="J334">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="K334">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="L334">
+            <v>0.26126009934648597</v>
+          </cell>
+        </row>
+        <row r="335">
+          <cell r="E335">
+            <v>0.28376063517712863</v>
+          </cell>
+          <cell r="F335">
+            <v>0.28376063517712863</v>
+          </cell>
+          <cell r="G335">
+            <v>0.27125610556295471</v>
+          </cell>
+          <cell r="H335">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="I335">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="J335">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="K335">
+            <v>0.26126009934648597</v>
+          </cell>
+          <cell r="L335">
+            <v>0.26126009934648597</v>
+          </cell>
+        </row>
+        <row r="336">
+          <cell r="E336">
+            <v>0.29665884586699809</v>
+          </cell>
+          <cell r="F336">
+            <v>0.29665884586699809</v>
+          </cell>
+          <cell r="G336">
+            <v>0.27517153975168673</v>
+          </cell>
+          <cell r="H336">
+            <v>0.26107366116029451</v>
+          </cell>
+          <cell r="I336">
+            <v>0.26107366116029451</v>
+          </cell>
+          <cell r="J336">
+            <v>0.26107366116029451</v>
+          </cell>
+          <cell r="K336">
+            <v>0.26107366116029451</v>
+          </cell>
+          <cell r="L336">
+            <v>0.26107366116029451</v>
+          </cell>
+        </row>
+        <row r="337">
+          <cell r="E337">
+            <v>1.0194657527051727</v>
+          </cell>
+          <cell r="F337">
+            <v>1.0194657527051727</v>
+          </cell>
+          <cell r="G337">
+            <v>1.0194657527051727</v>
+          </cell>
+          <cell r="H337">
+            <v>1.0194657527051727</v>
+          </cell>
+          <cell r="I337">
+            <v>1.0194657527051727</v>
+          </cell>
+          <cell r="J337">
+            <v>1.0194657527051727</v>
+          </cell>
+          <cell r="K337">
+            <v>1.0194657527051727</v>
+          </cell>
+          <cell r="L337">
+            <v>1.0194657527051727</v>
+          </cell>
+        </row>
+        <row r="338">
+          <cell r="E338">
+            <v>1.1844945352304528</v>
+          </cell>
+          <cell r="F338">
+            <v>1.1844945352304528</v>
+          </cell>
+          <cell r="G338">
+            <v>1.0987003746146558</v>
+          </cell>
+          <cell r="H338">
+            <v>1.019120373521627</v>
+          </cell>
+          <cell r="I338">
+            <v>1.019120373521627</v>
+          </cell>
+          <cell r="J338">
+            <v>1.019120373521627</v>
+          </cell>
+          <cell r="K338">
+            <v>1.019120373521627</v>
+          </cell>
+          <cell r="L338">
+            <v>1.019120373521627</v>
+          </cell>
+        </row>
+        <row r="339">
+          <cell r="E339">
+            <v>1.0704390403404314</v>
+          </cell>
+          <cell r="F339">
+            <v>1.0704390403404314</v>
+          </cell>
+          <cell r="G339">
+            <v>1.0387715804049205</v>
+          </cell>
+          <cell r="H339">
+            <v>1.0202299404292809</v>
+          </cell>
+          <cell r="I339">
+            <v>1.0202299404292809</v>
+          </cell>
+          <cell r="J339">
+            <v>1.0202299404292809</v>
+          </cell>
+          <cell r="K339">
+            <v>1.0202299404292809</v>
+          </cell>
+          <cell r="L339">
+            <v>1.0202299404292809</v>
+          </cell>
+        </row>
+        <row r="340">
+          <cell r="E340">
+            <v>1.1723856156109485</v>
+          </cell>
+          <cell r="F340">
+            <v>1.1723856156109485</v>
+          </cell>
+          <cell r="G340">
+            <v>1.0874685165296882</v>
+          </cell>
+          <cell r="H340">
+            <v>1.0209360082276679</v>
+          </cell>
+          <cell r="I340">
+            <v>1.0209360082276679</v>
+          </cell>
+          <cell r="J340">
+            <v>1.0209360082276679</v>
+          </cell>
+          <cell r="K340">
+            <v>1.0209360082276679</v>
+          </cell>
+          <cell r="L340">
+            <v>1.0209360082276679</v>
+          </cell>
+        </row>
+        <row r="619">
+          <cell r="E619">
+            <v>1990</v>
+          </cell>
+          <cell r="F619">
+            <v>2005</v>
+          </cell>
+          <cell r="G619">
+            <v>2020</v>
+          </cell>
+          <cell r="H619">
+            <v>2035</v>
+          </cell>
+          <cell r="I619">
+            <v>2050</v>
+          </cell>
+          <cell r="J619">
+            <v>2065</v>
+          </cell>
+          <cell r="K619">
+            <v>2080</v>
+          </cell>
+          <cell r="L619">
+            <v>2095</v>
+          </cell>
+        </row>
+        <row r="620">
+          <cell r="E620">
+            <v>27.622356387579874</v>
+          </cell>
+          <cell r="F620">
+            <v>27.622356387579874</v>
+          </cell>
+          <cell r="G620">
+            <v>27.622356387579874</v>
+          </cell>
+          <cell r="H620">
+            <v>27.622356387579874</v>
+          </cell>
+          <cell r="I620">
+            <v>27.622356387579874</v>
+          </cell>
+          <cell r="J620">
+            <v>27.622356387579874</v>
+          </cell>
+          <cell r="K620">
+            <v>27.622356387579874</v>
+          </cell>
+          <cell r="L620">
+            <v>27.622356387579874</v>
+          </cell>
+        </row>
+        <row r="621">
+          <cell r="E621">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="F621">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="G621">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="H621">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="I621">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="J621">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="K621">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="L621">
+            <v>40.808519140991372</v>
+          </cell>
+        </row>
+        <row r="622">
+          <cell r="E622">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="F622">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="G622">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="H622">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="I622">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="J622">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="K622">
+            <v>40.808519140991372</v>
+          </cell>
+          <cell r="L622">
+            <v>40.808519140991372</v>
+          </cell>
+        </row>
+        <row r="623">
+          <cell r="E623">
+            <v>5.1108426086945284</v>
+          </cell>
+          <cell r="F623">
+            <v>5.1108426086945284</v>
+          </cell>
+          <cell r="G623">
+            <v>5.1108426086945284</v>
+          </cell>
+          <cell r="H623">
+            <v>5.1108426086945284</v>
+          </cell>
+          <cell r="I623">
+            <v>5.1108426086945284</v>
+          </cell>
+          <cell r="J623">
+            <v>5.1108426086945284</v>
+          </cell>
+          <cell r="K623">
+            <v>5.1108426086945284</v>
+          </cell>
+          <cell r="L623">
+            <v>5.1108426086945284</v>
+          </cell>
+        </row>
+        <row r="624">
+          <cell r="E624">
+            <v>1000</v>
+          </cell>
+          <cell r="F624">
+            <v>1000</v>
+          </cell>
+          <cell r="G624">
+            <v>1000</v>
+          </cell>
+          <cell r="H624">
+            <v>1000</v>
+          </cell>
+          <cell r="I624">
+            <v>1000</v>
+          </cell>
+          <cell r="J624">
+            <v>1000</v>
+          </cell>
+          <cell r="K624">
+            <v>1000</v>
+          </cell>
+          <cell r="L624">
+            <v>1000</v>
+          </cell>
+        </row>
+        <row r="625">
+          <cell r="E625">
+            <v>123.7391147374434</v>
+          </cell>
+          <cell r="F625">
+            <v>123.7391147374434</v>
+          </cell>
+          <cell r="G625">
+            <v>123.7391147374434</v>
+          </cell>
+          <cell r="H625">
+            <v>123.7391147374434</v>
+          </cell>
+          <cell r="I625">
+            <v>123.7391147374434</v>
+          </cell>
+          <cell r="J625">
+            <v>123.7391147374434</v>
+          </cell>
+          <cell r="K625">
+            <v>123.7391147374434</v>
+          </cell>
+          <cell r="L625">
+            <v>123.7391147374434</v>
+          </cell>
+        </row>
+        <row r="626">
+          <cell r="E626">
+            <v>310.33333333333331</v>
+          </cell>
+          <cell r="F626">
+            <v>310.33333333333331</v>
+          </cell>
+          <cell r="G626">
+            <v>310.33333333333331</v>
+          </cell>
+          <cell r="H626">
+            <v>310.33333333333331</v>
+          </cell>
+          <cell r="I626">
+            <v>310.33333333333331</v>
+          </cell>
+          <cell r="J626">
+            <v>310.33333333333331</v>
+          </cell>
+          <cell r="K626">
+            <v>310.33333333333331</v>
+          </cell>
+          <cell r="L626">
+            <v>310.33333333333331</v>
+          </cell>
+        </row>
+        <row r="627">
+          <cell r="E627">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="F627">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="G627">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="H627">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="I627">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="J627">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="K627">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="L627">
+            <v>25.316589215566697</v>
+          </cell>
+        </row>
+        <row r="628">
+          <cell r="E628">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="F628">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="G628">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="H628">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="I628">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="J628">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="K628">
+            <v>25.316589215566697</v>
+          </cell>
+          <cell r="L628">
+            <v>25.316589215566697</v>
+          </cell>
+        </row>
+        <row r="629">
+          <cell r="E629">
+            <v>19448.634706025085</v>
+          </cell>
+          <cell r="F629">
+            <v>19448.634706025085</v>
+          </cell>
+          <cell r="G629">
+            <v>19448.634706025085</v>
+          </cell>
+          <cell r="H629">
+            <v>19448.634706025085</v>
+          </cell>
+          <cell r="I629">
+            <v>19448.634706025085</v>
+          </cell>
+          <cell r="J629">
+            <v>19448.634706025085</v>
+          </cell>
+          <cell r="K629">
+            <v>19448.634706025085</v>
+          </cell>
+          <cell r="L629">
+            <v>19448.634706025085</v>
+          </cell>
+        </row>
+        <row r="630">
+          <cell r="E630">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="F630">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="G630">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="H630">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="I630">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="J630">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="K630">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="L630">
+            <v>1.6309764579543651</v>
+          </cell>
+        </row>
+        <row r="631">
+          <cell r="E631">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="F631">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="G631">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="H631">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="I631">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="J631">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="K631">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="L631">
+            <v>1.6309764579543651</v>
+          </cell>
+        </row>
+        <row r="632">
+          <cell r="E632">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="F632">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="G632">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="H632">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="I632">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="J632">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="K632">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="L632">
+            <v>1.6309764579543651</v>
+          </cell>
+        </row>
+        <row r="633">
+          <cell r="E633">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="F633">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="G633">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="H633">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="I633">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="J633">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="K633">
+            <v>1.6309764579543651</v>
+          </cell>
+          <cell r="L633">
+            <v>1.6309764579543651</v>
+          </cell>
+        </row>
+        <row r="634">
+          <cell r="E634">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="F634">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="G634">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="H634">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="I634">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="J634">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="K634">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="L634">
+            <v>18.861799866247672</v>
+          </cell>
+        </row>
+        <row r="635">
+          <cell r="E635">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="F635">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="G635">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="H635">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="I635">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="J635">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="K635">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="L635">
+            <v>18.861799866247672</v>
+          </cell>
+        </row>
+        <row r="636">
+          <cell r="E636">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="F636">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="G636">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="H636">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="I636">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="J636">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="K636">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="L636">
+            <v>18.861799866247672</v>
+          </cell>
+        </row>
+        <row r="637">
+          <cell r="E637">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="F637">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="G637">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="H637">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="I637">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="J637">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="K637">
+            <v>18.861799866247672</v>
+          </cell>
+          <cell r="L637">
+            <v>18.861799866247672</v>
+          </cell>
+        </row>
+        <row r="919">
+          <cell r="E919">
+            <v>2020</v>
+          </cell>
+          <cell r="F919">
+            <v>2035</v>
+          </cell>
+          <cell r="G919">
+            <v>2050</v>
+          </cell>
+          <cell r="H919">
+            <v>2065</v>
+          </cell>
+          <cell r="I919">
+            <v>2080</v>
+          </cell>
+          <cell r="J919">
+            <v>2095</v>
+          </cell>
+        </row>
+        <row r="920">
+          <cell r="E920">
+            <v>1</v>
+          </cell>
+          <cell r="F920">
+            <v>1</v>
+          </cell>
+          <cell r="G920">
+            <v>1</v>
+          </cell>
+          <cell r="H920">
+            <v>1</v>
+          </cell>
+          <cell r="I920">
+            <v>1</v>
+          </cell>
+          <cell r="J920">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="921">
+          <cell r="E921">
+            <v>1</v>
+          </cell>
+          <cell r="F921">
+            <v>1</v>
+          </cell>
+          <cell r="G921">
+            <v>1</v>
+          </cell>
+          <cell r="H921">
+            <v>1</v>
+          </cell>
+          <cell r="I921">
+            <v>1</v>
+          </cell>
+          <cell r="J921">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="922">
+          <cell r="E922">
+            <v>0.1</v>
+          </cell>
+          <cell r="F922">
+            <v>0.25</v>
+          </cell>
+          <cell r="G922">
+            <v>0.5</v>
+          </cell>
+          <cell r="H922">
+            <v>0.5</v>
+          </cell>
+          <cell r="I922">
+            <v>0.5</v>
+          </cell>
+          <cell r="J922">
+            <v>0.5</v>
+          </cell>
+        </row>
+        <row r="923">
+          <cell r="E923">
+            <v>1</v>
+          </cell>
+          <cell r="F923">
+            <v>1</v>
+          </cell>
+          <cell r="G923">
+            <v>1</v>
+          </cell>
+          <cell r="H923">
+            <v>1</v>
+          </cell>
+          <cell r="I923">
+            <v>1</v>
+          </cell>
+          <cell r="J923">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="924">
+          <cell r="E924">
+            <v>1</v>
+          </cell>
+          <cell r="F924">
+            <v>1</v>
+          </cell>
+          <cell r="G924">
+            <v>1</v>
+          </cell>
+          <cell r="H924">
+            <v>1</v>
+          </cell>
+          <cell r="I924">
+            <v>1</v>
+          </cell>
+          <cell r="J924">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="925">
+          <cell r="E925">
+            <v>1</v>
+          </cell>
+          <cell r="F925">
+            <v>1</v>
+          </cell>
+          <cell r="G925">
+            <v>1</v>
+          </cell>
+          <cell r="H925">
+            <v>1</v>
+          </cell>
+          <cell r="I925">
+            <v>1</v>
+          </cell>
+          <cell r="J925">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="926">
+          <cell r="E926">
+            <v>0.1</v>
+          </cell>
+          <cell r="F926">
+            <v>0.25</v>
+          </cell>
+          <cell r="G926">
+            <v>0.5</v>
+          </cell>
+          <cell r="H926">
+            <v>0.5</v>
+          </cell>
+          <cell r="I926">
+            <v>0.5</v>
+          </cell>
+          <cell r="J926">
+            <v>0.5</v>
+          </cell>
+        </row>
+        <row r="927">
+          <cell r="E927">
+            <v>1</v>
+          </cell>
+          <cell r="F927">
+            <v>1</v>
+          </cell>
+          <cell r="G927">
+            <v>1</v>
+          </cell>
+          <cell r="H927">
+            <v>1</v>
+          </cell>
+          <cell r="I927">
+            <v>1</v>
+          </cell>
+          <cell r="J927">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="928">
+          <cell r="E928">
+            <v>1</v>
+          </cell>
+          <cell r="F928">
+            <v>1</v>
+          </cell>
+          <cell r="G928">
+            <v>1</v>
+          </cell>
+          <cell r="H928">
+            <v>1</v>
+          </cell>
+          <cell r="I928">
+            <v>1</v>
+          </cell>
+          <cell r="J928">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="929">
+          <cell r="E929">
+            <v>1</v>
+          </cell>
+          <cell r="F929">
+            <v>1</v>
+          </cell>
+          <cell r="G929">
+            <v>1</v>
+          </cell>
+          <cell r="H929">
+            <v>1</v>
+          </cell>
+          <cell r="I929">
+            <v>1</v>
+          </cell>
+          <cell r="J929">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="930">
+          <cell r="E930">
+            <v>1</v>
+          </cell>
+          <cell r="F930">
+            <v>1</v>
+          </cell>
+          <cell r="G930">
+            <v>1</v>
+          </cell>
+          <cell r="H930">
+            <v>1</v>
+          </cell>
+          <cell r="I930">
+            <v>1</v>
+          </cell>
+          <cell r="J930">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="931">
+          <cell r="E931">
+            <v>0.1</v>
+          </cell>
+          <cell r="F931">
+            <v>0.25</v>
+          </cell>
+          <cell r="G931">
+            <v>0.5</v>
+          </cell>
+          <cell r="H931">
+            <v>0.5</v>
+          </cell>
+          <cell r="I931">
+            <v>0.5</v>
+          </cell>
+          <cell r="J931">
+            <v>0.5</v>
+          </cell>
+        </row>
+        <row r="932">
+          <cell r="E932">
+            <v>0.01</v>
+          </cell>
+          <cell r="F932">
+            <v>0.1</v>
+          </cell>
+          <cell r="G932">
+            <v>0.25</v>
+          </cell>
+          <cell r="H932">
+            <v>0.25</v>
+          </cell>
+          <cell r="I932">
+            <v>0.25</v>
+          </cell>
+          <cell r="J932">
+            <v>0.25</v>
+          </cell>
+        </row>
+        <row r="933">
+          <cell r="E933">
+            <v>0</v>
+          </cell>
+          <cell r="F933">
+            <v>0.1</v>
+          </cell>
+          <cell r="G933">
+            <v>0.25</v>
+          </cell>
+          <cell r="H933">
+            <v>0.25</v>
+          </cell>
+          <cell r="I933">
+            <v>0.25</v>
+          </cell>
+          <cell r="J933">
+            <v>0.25</v>
+          </cell>
+        </row>
+        <row r="934">
+          <cell r="E934">
+            <v>1</v>
+          </cell>
+          <cell r="F934">
+            <v>1</v>
+          </cell>
+          <cell r="G934">
+            <v>1</v>
+          </cell>
+          <cell r="H934">
+            <v>1</v>
+          </cell>
+          <cell r="I934">
+            <v>1</v>
+          </cell>
+          <cell r="J934">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="935">
+          <cell r="E935">
+            <v>0.1</v>
+          </cell>
+          <cell r="F935">
+            <v>0.25</v>
+          </cell>
+          <cell r="G935">
+            <v>0.5</v>
+          </cell>
+          <cell r="H935">
+            <v>0.5</v>
+          </cell>
+          <cell r="I935">
+            <v>0.5</v>
+          </cell>
+          <cell r="J935">
+            <v>0.5</v>
+          </cell>
+        </row>
+        <row r="936">
+          <cell r="E936">
+            <v>1</v>
+          </cell>
+          <cell r="F936">
+            <v>1</v>
+          </cell>
+          <cell r="G936">
+            <v>1</v>
+          </cell>
+          <cell r="H936">
+            <v>1</v>
+          </cell>
+          <cell r="I936">
+            <v>1</v>
+          </cell>
+          <cell r="J936">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="937">
+          <cell r="E937">
+            <v>0.1</v>
+          </cell>
+          <cell r="F937">
+            <v>0.25</v>
+          </cell>
+          <cell r="G937">
+            <v>0.5</v>
+          </cell>
+          <cell r="H937">
+            <v>0.5</v>
+          </cell>
+          <cell r="I937">
+            <v>0.5</v>
+          </cell>
+          <cell r="J937">
+            <v>0.5</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6368,6 +8468,1388 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="str">
+        <f>Legend!A$38</f>
+        <v>trn_freight</v>
+      </c>
+      <c r="B4" t="str">
+        <f>Legend!B$38</f>
+        <v>rail</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Legend!C$38</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D4" s="12">
+        <v>2020</v>
+      </c>
+      <c r="E4">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K4,MATCH($D4,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K4,MATCH($D4,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>2841.7305800733889</v>
+      </c>
+      <c r="G4">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K4,MATCH($D4,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.45279314957056366</v>
+      </c>
+      <c r="H4">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K4,MATCH($D4,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>40.808519140991372</v>
+      </c>
+      <c r="I4" t="str">
+        <f>Legend!D$38</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <f t="array" ref="K4:K33">MATCH(CONCATENATE($A$4:$A$33,$C$4:$C$33),CONCATENATE([1]global_det_trn_adv!$B$25:$B$42,[1]global_det_trn_adv!$D$25:$D$42),FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="str">
+        <f>Legend!A$38</f>
+        <v>trn_freight</v>
+      </c>
+      <c r="B5" t="str">
+        <f>Legend!B$38</f>
+        <v>rail</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Legend!C$38</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" ref="D5:D9" si="0">D4+15</f>
+        <v>2035</v>
+      </c>
+      <c r="E5">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K5,MATCH($D5,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.25</v>
+      </c>
+      <c r="F5">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K5,MATCH($D5,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>2737.0105167775223</v>
+      </c>
+      <c r="G5">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K5,MATCH($D5,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.43283983453669406</v>
+      </c>
+      <c r="H5">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K5,MATCH($D5,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>40.808519140991372</v>
+      </c>
+      <c r="I5" t="str">
+        <f>Legend!D$38</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="str">
+        <f>Legend!A$38</f>
+        <v>trn_freight</v>
+      </c>
+      <c r="B6" t="str">
+        <f>Legend!B$38</f>
+        <v>rail</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Legend!C$38</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="E6">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K6,MATCH($D6,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F6">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K6,MATCH($D6,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>2636.1494722547891</v>
+      </c>
+      <c r="G6">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K6,MATCH($D6,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.43283983453669406</v>
+      </c>
+      <c r="H6">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K6,MATCH($D6,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>40.808519140991372</v>
+      </c>
+      <c r="I6" t="str">
+        <f>Legend!D$38</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="str">
+        <f>Legend!A$38</f>
+        <v>trn_freight</v>
+      </c>
+      <c r="B7" t="str">
+        <f>Legend!B$38</f>
+        <v>rail</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Legend!C$38</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="0"/>
+        <v>2065</v>
+      </c>
+      <c r="E7">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K7,MATCH($D7,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K7,MATCH($D7,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>2539.0052385516919</v>
+      </c>
+      <c r="G7">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K7,MATCH($D7,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.43283983453669406</v>
+      </c>
+      <c r="H7">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K7,MATCH($D7,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>40.808519140991372</v>
+      </c>
+      <c r="I7" t="str">
+        <f>Legend!D$38</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="str">
+        <f>Legend!A$38</f>
+        <v>trn_freight</v>
+      </c>
+      <c r="B8" t="str">
+        <f>Legend!B$38</f>
+        <v>rail</v>
+      </c>
+      <c r="C8" t="str">
+        <f>Legend!C$38</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="0"/>
+        <v>2080</v>
+      </c>
+      <c r="E8">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K8,MATCH($D8,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K8,MATCH($D8,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>2445.4408481924893</v>
+      </c>
+      <c r="G8">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K8,MATCH($D8,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.43283983453669406</v>
+      </c>
+      <c r="H8">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K8,MATCH($D8,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>40.808519140991372</v>
+      </c>
+      <c r="I8" t="str">
+        <f>Legend!D$38</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="str">
+        <f>Legend!A$38</f>
+        <v>trn_freight</v>
+      </c>
+      <c r="B9" t="str">
+        <f>Legend!B$38</f>
+        <v>rail</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Legend!C$38</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="0"/>
+        <v>2095</v>
+      </c>
+      <c r="E9">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K9,MATCH($D9,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F9">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K9,MATCH($D9,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>2355.3243810633635</v>
+      </c>
+      <c r="G9">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K9,MATCH($D9,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.43283983453669406</v>
+      </c>
+      <c r="H9">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K9,MATCH($D9,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>40.808519140991372</v>
+      </c>
+      <c r="I9" t="str">
+        <f>Legend!D$38</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="str">
+        <f>Legend!A$42</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B10" t="str">
+        <f>Legend!B$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="C10" t="str">
+        <f>Legend!C$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2020</v>
+      </c>
+      <c r="E10">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K10,MATCH($D10,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="F10">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K10,MATCH($D10,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>109438.81879413639</v>
+      </c>
+      <c r="G10">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K10,MATCH($D10,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>31.0069897367297</v>
+      </c>
+      <c r="H10">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K10,MATCH($D10,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>310.33333333333331</v>
+      </c>
+      <c r="I10" t="str">
+        <f>Legend!D$42</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="str">
+        <f>Legend!A$42</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B11" t="str">
+        <f>Legend!B$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Legend!C$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" ref="D11:D15" si="1">D10+15</f>
+        <v>2035</v>
+      </c>
+      <c r="E11">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K11,MATCH($D11,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.25</v>
+      </c>
+      <c r="F11">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K11,MATCH($D11,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>105405.91007593874</v>
+      </c>
+      <c r="G11">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K11,MATCH($D11,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>30.545126558652367</v>
+      </c>
+      <c r="H11">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K11,MATCH($D11,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>310.33333333333331</v>
+      </c>
+      <c r="I11" t="str">
+        <f>Legend!D$42</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="str">
+        <f>Legend!A$42</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B12" t="str">
+        <f>Legend!B$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="C12" t="str">
+        <f>Legend!C$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="1"/>
+        <v>2050</v>
+      </c>
+      <c r="E12">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K12,MATCH($D12,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K12,MATCH($D12,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>101521.61729592942</v>
+      </c>
+      <c r="G12">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K12,MATCH($D12,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>30.090143042131182</v>
+      </c>
+      <c r="H12">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K12,MATCH($D12,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>310.33333333333331</v>
+      </c>
+      <c r="I12" t="str">
+        <f>Legend!D$42</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="str">
+        <f>Legend!A$42</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B13" t="str">
+        <f>Legend!B$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Legend!C$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="1"/>
+        <v>2065</v>
+      </c>
+      <c r="E13">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K13,MATCH($D13,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K13,MATCH($D13,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>97780.463836950235</v>
+      </c>
+      <c r="G13">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K13,MATCH($D13,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>29.641936711486391</v>
+      </c>
+      <c r="H13">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K13,MATCH($D13,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>310.33333333333331</v>
+      </c>
+      <c r="I13" t="str">
+        <f>Legend!D$42</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="str">
+        <f>Legend!A$42</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B14" t="str">
+        <f>Legend!B$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="C14" t="str">
+        <f>Legend!C$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="1"/>
+        <v>2080</v>
+      </c>
+      <c r="E14">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K14,MATCH($D14,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F14">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K14,MATCH($D14,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>94177.17489960129</v>
+      </c>
+      <c r="G14">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K14,MATCH($D14,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>29.200406617459976</v>
+      </c>
+      <c r="H14">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K14,MATCH($D14,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>310.33333333333331</v>
+      </c>
+      <c r="I14" t="str">
+        <f>Legend!D$42</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="str">
+        <f>Legend!A$42</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B15" t="str">
+        <f>Legend!B$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Legend!C$42</f>
+        <v>high speed rail</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="1"/>
+        <v>2095</v>
+      </c>
+      <c r="E15">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K15,MATCH($D15,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F15">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K15,MATCH($D15,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>90706.670065093916</v>
+      </c>
+      <c r="G15">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K15,MATCH($D15,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>28.765453314478911</v>
+      </c>
+      <c r="H15">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K15,MATCH($D15,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>310.33333333333331</v>
+      </c>
+      <c r="I15" t="str">
+        <f>Legend!D$42</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="str">
+        <f>Legend!A$45</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B16" t="str">
+        <f>Legend!B$45</f>
+        <v>rail</v>
+      </c>
+      <c r="C16" t="str">
+        <f>Legend!C$45</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2020</v>
+      </c>
+      <c r="E16">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K16,MATCH($D16,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K16,MATCH($D16,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>14012.724712768266</v>
+      </c>
+      <c r="G16">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K16,MATCH($D16,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.759574734708778</v>
+      </c>
+      <c r="H16">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K16,MATCH($D16,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>25.316589215566697</v>
+      </c>
+      <c r="I16" t="str">
+        <f>Legend!D$45</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="str">
+        <f>Legend!A$45</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B17" t="str">
+        <f>Legend!B$45</f>
+        <v>rail</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Legend!C$45</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" ref="D17:D21" si="2">D16+15</f>
+        <v>2035</v>
+      </c>
+      <c r="E17">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K17,MATCH($D17,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K17,MATCH($D17,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>13496.344507987997</v>
+      </c>
+      <c r="G17">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K17,MATCH($D17,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.759574734708778</v>
+      </c>
+      <c r="H17">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K17,MATCH($D17,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>25.316589215566697</v>
+      </c>
+      <c r="I17" t="str">
+        <f>Legend!D$45</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="str">
+        <f>Legend!A$45</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B18" t="str">
+        <f>Legend!B$45</f>
+        <v>rail</v>
+      </c>
+      <c r="C18" t="str">
+        <f>Legend!C$45</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="2"/>
+        <v>2050</v>
+      </c>
+      <c r="E18">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K18,MATCH($D18,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K18,MATCH($D18,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>12998.99333013537</v>
+      </c>
+      <c r="G18">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K18,MATCH($D18,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.759574734708778</v>
+      </c>
+      <c r="H18">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K18,MATCH($D18,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>25.316589215566697</v>
+      </c>
+      <c r="I18" t="str">
+        <f>Legend!D$45</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="str">
+        <f>Legend!A$45</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B19" t="str">
+        <f>Legend!B$45</f>
+        <v>rail</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Legend!C$45</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="2"/>
+        <v>2065</v>
+      </c>
+      <c r="E19">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K19,MATCH($D19,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K19,MATCH($D19,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>12519.969944224109</v>
+      </c>
+      <c r="G19">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K19,MATCH($D19,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.759574734708778</v>
+      </c>
+      <c r="H19">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K19,MATCH($D19,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>25.316589215566697</v>
+      </c>
+      <c r="I19" t="str">
+        <f>Legend!D$45</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="str">
+        <f>Legend!A$45</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B20" t="str">
+        <f>Legend!B$45</f>
+        <v>rail</v>
+      </c>
+      <c r="C20" t="str">
+        <f>Legend!C$45</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D20" s="12">
+        <f t="shared" si="2"/>
+        <v>2080</v>
+      </c>
+      <c r="E20">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K20,MATCH($D20,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K20,MATCH($D20,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>12058.598956342619</v>
+      </c>
+      <c r="G20">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K20,MATCH($D20,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.759574734708778</v>
+      </c>
+      <c r="H20">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K20,MATCH($D20,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>25.316589215566697</v>
+      </c>
+      <c r="I20" t="str">
+        <f>Legend!D$45</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="str">
+        <f>Legend!A$45</f>
+        <v>trn_passenger</v>
+      </c>
+      <c r="B21" t="str">
+        <f>Legend!B$45</f>
+        <v>rail</v>
+      </c>
+      <c r="C21" t="str">
+        <f>Legend!C$45</f>
+        <v>rail electric</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="2"/>
+        <v>2095</v>
+      </c>
+      <c r="E21">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K21,MATCH($D21,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K21,MATCH($D21,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>11614.229861389551</v>
+      </c>
+      <c r="G21">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K21,MATCH($D21,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.759574734708778</v>
+      </c>
+      <c r="H21">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K21,MATCH($D21,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>25.316589215566697</v>
+      </c>
+      <c r="I21" t="str">
+        <f>Legend!D$45</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="str">
+        <f>Legend!A$54</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B22" t="str">
+        <f>Legend!B$54</f>
+        <v>LDV</v>
+      </c>
+      <c r="C22" t="str">
+        <f>Legend!C$54</f>
+        <v>LDV electric</v>
+      </c>
+      <c r="D22" s="12">
+        <v>2020</v>
+      </c>
+      <c r="E22">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K22,MATCH($D22,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="F22">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K22,MATCH($D22,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>1132.2394866886907</v>
+      </c>
+      <c r="G22">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K22,MATCH($D22,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.27125610556295471</v>
+      </c>
+      <c r="H22">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K22,MATCH($D22,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>1.6309764579543651</v>
+      </c>
+      <c r="I22" t="str">
+        <f>Legend!D$54</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="str">
+        <f>Legend!A$54</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B23" t="str">
+        <f>Legend!B$54</f>
+        <v>LDV</v>
+      </c>
+      <c r="C23" t="str">
+        <f>Legend!C$54</f>
+        <v>LDV electric</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" ref="D23:D26" si="3">D22+15</f>
+        <v>2035</v>
+      </c>
+      <c r="E23">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K23,MATCH($D23,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.25</v>
+      </c>
+      <c r="F23">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K23,MATCH($D23,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>1066.1747012022947</v>
+      </c>
+      <c r="G23">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K23,MATCH($D23,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.26126009934648597</v>
+      </c>
+      <c r="H23">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K23,MATCH($D23,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>1.6309764579543651</v>
+      </c>
+      <c r="I23" t="str">
+        <f>Legend!D$54</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J23" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="str">
+        <f>Legend!A$54</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B24" t="str">
+        <f>Legend!B$54</f>
+        <v>LDV</v>
+      </c>
+      <c r="C24" t="str">
+        <f>Legend!C$54</f>
+        <v>LDV electric</v>
+      </c>
+      <c r="D24" s="12">
+        <f t="shared" si="3"/>
+        <v>2050</v>
+      </c>
+      <c r="E24">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K24,MATCH($D24,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F24">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K24,MATCH($D24,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>1003.9647149281467</v>
+      </c>
+      <c r="G24">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K24,MATCH($D24,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.26126009934648597</v>
+      </c>
+      <c r="H24">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K24,MATCH($D24,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>1.6309764579543651</v>
+      </c>
+      <c r="I24" t="str">
+        <f>Legend!D$54</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="str">
+        <f>Legend!A$54</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B25" t="str">
+        <f>Legend!B$54</f>
+        <v>LDV</v>
+      </c>
+      <c r="C25" t="str">
+        <f>Legend!C$54</f>
+        <v>LDV electric</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" si="3"/>
+        <v>2065</v>
+      </c>
+      <c r="E25">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K25,MATCH($D25,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F25">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K25,MATCH($D25,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>945.38460505968101</v>
+      </c>
+      <c r="G25">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K25,MATCH($D25,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.26126009934648597</v>
+      </c>
+      <c r="H25">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K25,MATCH($D25,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>1.6309764579543651</v>
+      </c>
+      <c r="I25" t="str">
+        <f>Legend!D$54</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J25" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="str">
+        <f>Legend!A$54</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B26" t="str">
+        <f>Legend!B$54</f>
+        <v>LDV</v>
+      </c>
+      <c r="C26" t="str">
+        <f>Legend!C$54</f>
+        <v>LDV electric</v>
+      </c>
+      <c r="D26" s="12">
+        <f t="shared" si="3"/>
+        <v>2080</v>
+      </c>
+      <c r="E26">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K26,MATCH($D26,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F26">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K26,MATCH($D26,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>890.22257276025334</v>
+      </c>
+      <c r="G26">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K26,MATCH($D26,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.26126009934648597</v>
+      </c>
+      <c r="H26">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K26,MATCH($D26,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>1.6309764579543651</v>
+      </c>
+      <c r="I26" t="str">
+        <f>Legend!D$54</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="str">
+        <f>Legend!A$54</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B27" t="str">
+        <f>Legend!B$54</f>
+        <v>LDV</v>
+      </c>
+      <c r="C27" t="str">
+        <f>Legend!C$54</f>
+        <v>LDV electric</v>
+      </c>
+      <c r="D27" s="12">
+        <f>D26+15</f>
+        <v>2095</v>
+      </c>
+      <c r="E27">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K27,MATCH($D27,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F27">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K27,MATCH($D27,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>838.27917739559041</v>
+      </c>
+      <c r="G27">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K27,MATCH($D27,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>0.26126009934648597</v>
+      </c>
+      <c r="H27">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K27,MATCH($D27,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>1.6309764579543651</v>
+      </c>
+      <c r="I27" t="str">
+        <f>Legend!D$54</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="str">
+        <f>Legend!A$58</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B28" t="str">
+        <f>Legend!B$58</f>
+        <v>bus</v>
+      </c>
+      <c r="C28" t="str">
+        <f>Legend!C$58</f>
+        <v>bus electric</v>
+      </c>
+      <c r="D28" s="12">
+        <v>2020</v>
+      </c>
+      <c r="E28">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K28,MATCH($D28,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="F28">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K28,MATCH($D28,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>4739.9138800913734</v>
+      </c>
+      <c r="G28">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K28,MATCH($D28,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.0987003746146558</v>
+      </c>
+      <c r="H28">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K28,MATCH($D28,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>18.861799866247672</v>
+      </c>
+      <c r="I28" t="str">
+        <f>Legend!D$58</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="str">
+        <f>Legend!A$58</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B29" t="str">
+        <f>Legend!B$58</f>
+        <v>bus</v>
+      </c>
+      <c r="C29" t="str">
+        <f>Legend!C$58</f>
+        <v>bus electric</v>
+      </c>
+      <c r="D29" s="12">
+        <f t="shared" ref="D29:D33" si="4">D28+15</f>
+        <v>2035</v>
+      </c>
+      <c r="E29">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K29,MATCH($D29,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.25</v>
+      </c>
+      <c r="F29">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K29,MATCH($D29,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>4463.3457181488593</v>
+      </c>
+      <c r="G29">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K29,MATCH($D29,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.019120373521627</v>
+      </c>
+      <c r="H29">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K29,MATCH($D29,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>18.861799866247672</v>
+      </c>
+      <c r="I29" t="str">
+        <f>Legend!D$58</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J29" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="str">
+        <f>Legend!A$58</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B30" t="str">
+        <f>Legend!B$58</f>
+        <v>bus</v>
+      </c>
+      <c r="C30" t="str">
+        <f>Legend!C$58</f>
+        <v>bus electric</v>
+      </c>
+      <c r="D30" s="12">
+        <f t="shared" si="4"/>
+        <v>2050</v>
+      </c>
+      <c r="E30">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K30,MATCH($D30,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F30">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K30,MATCH($D30,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>4202.9149692765559</v>
+      </c>
+      <c r="G30">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K30,MATCH($D30,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.019120373521627</v>
+      </c>
+      <c r="H30">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K30,MATCH($D30,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>18.861799866247672</v>
+      </c>
+      <c r="I30" t="str">
+        <f>Legend!D$58</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="str">
+        <f>Legend!A$58</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B31" t="str">
+        <f>Legend!B$58</f>
+        <v>bus</v>
+      </c>
+      <c r="C31" t="str">
+        <f>Legend!C$58</f>
+        <v>bus electric</v>
+      </c>
+      <c r="D31" s="12">
+        <f t="shared" si="4"/>
+        <v>2065</v>
+      </c>
+      <c r="E31">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K31,MATCH($D31,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F31">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K31,MATCH($D31,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>3957.6800352125033</v>
+      </c>
+      <c r="G31">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K31,MATCH($D31,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.019120373521627</v>
+      </c>
+      <c r="H31">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K31,MATCH($D31,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>18.861799866247672</v>
+      </c>
+      <c r="I31" t="str">
+        <f>Legend!D$58</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J31" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="str">
+        <f>Legend!A$58</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B32" t="str">
+        <f>Legend!B$58</f>
+        <v>bus</v>
+      </c>
+      <c r="C32" t="str">
+        <f>Legend!C$58</f>
+        <v>bus electric</v>
+      </c>
+      <c r="D32" s="12">
+        <f t="shared" si="4"/>
+        <v>2080</v>
+      </c>
+      <c r="E32">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K32,MATCH($D32,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F32">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K32,MATCH($D32,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>3726.754258798564</v>
+      </c>
+      <c r="G32">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K32,MATCH($D32,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.019120373521627</v>
+      </c>
+      <c r="H32">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K32,MATCH($D32,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>18.861799866247672</v>
+      </c>
+      <c r="I32" t="str">
+        <f>Legend!D$58</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="str">
+        <f>Legend!A$58</f>
+        <v>trn_pass_road</v>
+      </c>
+      <c r="B33" t="str">
+        <f>Legend!B$58</f>
+        <v>bus</v>
+      </c>
+      <c r="C33" t="str">
+        <f>Legend!C$58</f>
+        <v>bus electric</v>
+      </c>
+      <c r="D33" s="12">
+        <f t="shared" si="4"/>
+        <v>2095</v>
+      </c>
+      <c r="E33">
+        <f>INDEX([1]global_det_trn_adv!$E$920:$J$937,$K33,MATCH($D33,[1]global_det_trn_adv!$E$919:$J$919,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="F33">
+        <f>INDEX([1]global_det_trn_adv!$F$25:$N$42,$K33,MATCH($D33,[1]global_det_trn_adv!$F$24:$N$24,FALSE))</f>
+        <v>3509.3027182343949</v>
+      </c>
+      <c r="G33">
+        <f>INDEX([1]global_det_trn_adv!$E$323:$L$340,$K33,MATCH($D33,[1]global_det_trn_adv!$E$322:$L$322,FALSE))</f>
+        <v>1.019120373521627</v>
+      </c>
+      <c r="H33">
+        <f>INDEX([1]global_det_trn_adv!$E$620:$L$637,$K33,MATCH($D33,[1]global_det_trn_adv!$E$619:$L$619,FALSE))</f>
+        <v>18.861799866247672</v>
+      </c>
+      <c r="I33" t="str">
+        <f>Legend!D$58</f>
+        <v>elect_td_trn</v>
+      </c>
+      <c r="J33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
@@ -6450,7 +9932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -7801,7 +11283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>